<commit_message>
some key data filled in
</commit_message>
<xml_diff>
--- a/pitchTracking/keyData.xlsx
+++ b/pitchTracking/keyData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\Desktop\smc8-pm-project\workshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\Desktop\smc8-pm-project\pitchTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE595DB2-A987-4B2A-A943-B800AFC69DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD607B9-B2EC-4993-ADB8-624BF9CC8A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keynotes" sheetId="1" r:id="rId1"/>
+    <sheet name="raw" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="116">
   <si>
     <t>note</t>
   </si>
@@ -129,6 +130,261 @@
   </si>
   <si>
     <t>midi number</t>
+  </si>
+  <si>
+    <t>{'i': 0, 'avg': 27.981144915878772, 'med': 30.155607223510742}</t>
+  </si>
+  <si>
+    <t>{'i': 1, 'avg': 33.40596106090148, 'med': 33.98252868652344}</t>
+  </si>
+  <si>
+    <t>{'i': 2, 'avg': 31.30551833365361, 'med': 30.003725051879883}</t>
+  </si>
+  <si>
+    <t>{'i': 3, 'avg': 32.58934638798237, 'med': 32.52063751220703}</t>
+  </si>
+  <si>
+    <t>{'i': 4, 'avg': 34.437788217822714, 'med': 32.72134590148926}</t>
+  </si>
+  <si>
+    <t>{'i': 5, 'avg': 38.07692410155138, 'med': 38.558156967163086}</t>
+  </si>
+  <si>
+    <t>{'i': 6, 'avg': 40.099845308462776, 'med': 40.519195556640625}</t>
+  </si>
+  <si>
+    <t>{'i': 7, 'avg': 42.63179800963402, 'med': 42.90085220336914}</t>
+  </si>
+  <si>
+    <t>{'i': 8, 'avg': 46.087994646867116, 'med': 46.027334213256836}</t>
+  </si>
+  <si>
+    <t>{'i': 9, 'avg': 46.47803195973238, 'med': 46.51675033569336}</t>
+  </si>
+  <si>
+    <t>{'i': 10, 'avg': 52.01550079329809, 'med': 51.64544486999512}</t>
+  </si>
+  <si>
+    <t>{'i': 11, 'avg': 55.245900499343875, 'med': 54.68399429321289}</t>
+  </si>
+  <si>
+    <t>{'i': 12, 'avg': 58.33656443289916, 'med': 56.64212989807129}</t>
+  </si>
+  <si>
+    <t>{'i': 13, 'avg': 62.4422426028649, 'med': 63.860185623168945}</t>
+  </si>
+  <si>
+    <t>{'i': 14, 'avg': 66.75883223847548, 'med': 67.66460800170898}</t>
+  </si>
+  <si>
+    <t>{'i': 15, 'avg': 71.17297422854105, 'med': 71.3293228149414}</t>
+  </si>
+  <si>
+    <t>{'i': 16, 'avg': 75.71890605250995, 'med': 75.59438705444336}</t>
+  </si>
+  <si>
+    <t>{'i': 17, 'avg': 80.48422333105405, 'med': 80.52239227294922}</t>
+  </si>
+  <si>
+    <t>{'i': 18, 'avg': 85.65842625331878, 'med': 84.82609558105469}</t>
+  </si>
+  <si>
+    <t>{'i': 19, 'avg': 91.91957414428393, 'med': 90.39427185058594}</t>
+  </si>
+  <si>
+    <t>{'i': 20, 'avg': 98.53099295274417, 'med': 96.33784484863281}</t>
+  </si>
+  <si>
+    <t>{'i': 21, 'avg': 105.28279017869632, 'med': 107.48590087890625}</t>
+  </si>
+  <si>
+    <t>{'i': 22, 'avg': 112.70146010740598, 'med': 113.87747955322266}</t>
+  </si>
+  <si>
+    <t>{'i': 23, 'avg': 120.62661853528023, 'med': 120.64917755126953}</t>
+  </si>
+  <si>
+    <t>{'i': 24, 'avg': 127.3168320833842, 'med': 127.1151123046875}</t>
+  </si>
+  <si>
+    <t>{'i': 25, 'avg': 135.98563493378958, 'med': 136.17723083496094}</t>
+  </si>
+  <si>
+    <t>{'i': 26, 'avg': 144.39497889677685, 'med': 143.49569702148438}</t>
+  </si>
+  <si>
+    <t>{'i': 27, 'avg': 152.1852233265241, 'med': 149.2952423095703}</t>
+  </si>
+  <si>
+    <t>{'i': 28, 'avg': 163.9626669880549, 'med': 160.17417907714844}</t>
+  </si>
+  <si>
+    <t>{'i': 29, 'avg': 174.9157793334325, 'med': 177.6292495727539}</t>
+  </si>
+  <si>
+    <t>{'i': 30, 'avg': 188.08975978708267, 'med': 190.40322875976562}</t>
+  </si>
+  <si>
+    <t>{'i': 31, 'avg': 200.26188737503688, 'med': 200.57839965820312}</t>
+  </si>
+  <si>
+    <t>{'i': 32, 'avg': 213.6241743941307, 'med': 213.73367309570312}</t>
+  </si>
+  <si>
+    <t>{'i': 33, 'avg': 226.53191313028336, 'med': 226.45346069335938}</t>
+  </si>
+  <si>
+    <t>{'i': 34, 'avg': 241.7331495687167, 'med': 240.29383850097656}</t>
+  </si>
+  <si>
+    <t>{'i': 35, 'avg': 257.92340325069426, 'med': 252.74951934814453}</t>
+  </si>
+  <si>
+    <t>{'i': 36, 'avg': 275.970416208903, 'med': 271.1196594238281}</t>
+  </si>
+  <si>
+    <t>{'i': 37, 'avg': 294.11734366607664, 'med': 300.34690856933594}</t>
+  </si>
+  <si>
+    <t>{'i': 38, 'avg': 309.81862927246095, 'med': 312.6297912597656}</t>
+  </si>
+  <si>
+    <t>{'i': 39, 'avg': 340.29036672306063, 'med': 341.18994140625}</t>
+  </si>
+  <si>
+    <t>{'i': 40, 'avg': 359.0847039496104, 'med': 359.4280700683594}</t>
+  </si>
+  <si>
+    <t>{'i': 41, 'avg': 381.7346109647751, 'med': 380.9569549560547}</t>
+  </si>
+  <si>
+    <t>{'i': 42, 'avg': 405.82432209714256, 'med': 402.00999450683594}</t>
+  </si>
+  <si>
+    <t>{'i': 43, 'avg': 430.6718992621104, 'med': 422.7430114746094}</t>
+  </si>
+  <si>
+    <t>{'i': 44, 'avg': 465.6692874968847, 'med': 455.8449401855469}</t>
+  </si>
+  <si>
+    <t>{'i': 45, 'avg': 496.5378523429235, 'med': 503.2793273925781}</t>
+  </si>
+  <si>
+    <t>{'i': 46, 'avg': 516.9112265666325, 'med': 517.5404968261719}</t>
+  </si>
+  <si>
+    <t>{'i': 47, 'avg': 548.3527148876191, 'med': 548.1595153808594}</t>
+  </si>
+  <si>
+    <t>{'i': 48, 'avg': 595.4260498606363, 'med': 594.2708740234375}</t>
+  </si>
+  <si>
+    <t>{'i': 49, 'avg': 632.7552216008504, 'med': 632.917724609375}</t>
+  </si>
+  <si>
+    <t>{'i': 50, 'avg': 678.4946563739777, 'med': 671.1213073730469}</t>
+  </si>
+  <si>
+    <t>{'i': 51, 'avg': 724.9953222516377, 'med': 714.0751037597656}</t>
+  </si>
+  <si>
+    <t>{'i': 52, 'avg': 779.6351231320699, 'med': 798.4992370605469}</t>
+  </si>
+  <si>
+    <t>{'i': 53, 'avg': 837.2840430660248, 'med': 845.3357543945312}</t>
+  </si>
+  <si>
+    <t>{'i': 54, 'avg': 899.612169403712, 'med': 904.6489868164062}</t>
+  </si>
+  <si>
+    <t>{'i': 55, 'avg': 943.1841245765686, 'med': 943.7438659667969}</t>
+  </si>
+  <si>
+    <t>{'i': 56, 'avg': 1026.2843931007385, 'med': 1021.9467163085938}</t>
+  </si>
+  <si>
+    <t>{'i': 57, 'avg': 1085.865880575816, 'med': 1072.10888671875}</t>
+  </si>
+  <si>
+    <t>{'i': 58, 'avg': 1171.1091374193827, 'med': 1170.4387817382812}</t>
+  </si>
+  <si>
+    <t>{'i': 59, 'avg': 1251.5298928540549, 'med': 1270.192626953125}</t>
+  </si>
+  <si>
+    <t>{'i': 60, 'avg': 1337.5441422004699, 'med': 1337.2550048828125}</t>
+  </si>
+  <si>
+    <t>{'i': 61, 'avg': 1424.7448966255188, 'med': 1438.2018432617188}</t>
+  </si>
+  <si>
+    <t>{'i': 62, 'avg': 1532.4127755584716, 'med': 1529.1965942382812}</t>
+  </si>
+  <si>
+    <t>{'i': 63, 'avg': 1470.1853233954112, 'med': 1605.8682250976562}</t>
+  </si>
+  <si>
+    <t>{'i': 64, 'avg': 811.8186433175405, 'med': 742.8290710449219}</t>
+  </si>
+  <si>
+    <t>{'i': 65, 'avg': 1882.9552197113037, 'med': 1882.941650390625}</t>
+  </si>
+  <si>
+    <t>{'i': 66, 'avg': 2005.745669321696, 'med': 2005.4010620117188}</t>
+  </si>
+  <si>
+    <t>{'i': 67, 'avg': 2135.187772549947, 'med': 2141.633056640625}</t>
+  </si>
+  <si>
+    <t>{'i': 68, 'avg': 2217.460550804138, 'med': 2217.46044921875}</t>
+  </si>
+  <si>
+    <t>{'i': 69, 'avg': 2217.4604528427126, 'med': 2217.46044921875}</t>
+  </si>
+  <si>
+    <t>{'i': 70, 'avg': 2217.460440460205, 'med': 2217.46044921875}</t>
+  </si>
+  <si>
+    <t>{'i': 71, 'avg': 2217.4604576263428, 'med': 2217.46044921875}</t>
+  </si>
+  <si>
+    <t>{'i': 72, 'avg': 2217.460403625488, 'med': 2217.46044921875}</t>
+  </si>
+  <si>
+    <t>{'i': 73, 'avg': 2217.460412765503, 'med': 2217.46044921875}</t>
+  </si>
+  <si>
+    <t>{'i': 74, 'avg': 2217.46030683136, 'med': 2217.460205078125}</t>
+  </si>
+  <si>
+    <t>{'i': 75, 'avg': 2217.46039776357, 'med': 2217.46044921875}</t>
+  </si>
+  <si>
+    <t>{'i': 76, 'avg': 2217.4604235967, 'med': 2217.46044921875}</t>
+  </si>
+  <si>
+    <t>{'i': 77, 'avg': 2203.2891360905687, 'med': 2217.4561767578125}</t>
+  </si>
+  <si>
+    <t>{'i': 78, 'avg': nan, 'med': nan}</t>
+  </si>
+  <si>
+    <t>{'i': 79, 'avg': nan, 'med': nan}</t>
+  </si>
+  <si>
+    <t>{'i': 80, 'avg': nan, 'med': nan}</t>
+  </si>
+  <si>
+    <t>{'i': 81, 'avg': nan, 'med': nan}</t>
+  </si>
+  <si>
+    <t>{'i': 82, 'avg': nan, 'med': nan}</t>
+  </si>
+  <si>
+    <t>{'i': 83, 'avg': nan, 'med': nan}</t>
+  </si>
+  <si>
+    <t>{'i': 84, 'avg': nan, 'med': nan}</t>
   </si>
 </sst>
 </file>
@@ -136,7 +392,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -221,9 +477,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -506,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +874,7 @@
       </c>
       <c r="M2">
         <f ca="1">RAND()</f>
-        <v>0.21759427685774924</v>
+        <v>0.86313049722432511</v>
       </c>
       <c r="N2" s="7">
         <v>0.36363978468860625</v>
@@ -673,7 +929,7 @@
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M66" ca="1" si="5">RAND()</f>
-        <v>0.80070322324126808</v>
+        <v>0.78648795249160863</v>
       </c>
       <c r="N3" s="7">
         <v>0.15453078428827749</v>
@@ -728,7 +984,7 @@
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="5"/>
-        <v>0.42610748662676401</v>
+        <v>3.8783009174806926E-2</v>
       </c>
       <c r="N4" s="7">
         <v>0.65252324908191239</v>
@@ -783,7 +1039,7 @@
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48301442012791218</v>
+        <v>0.98948916576245471</v>
       </c>
       <c r="N5" s="7">
         <v>0.82101361555669505</v>
@@ -838,7 +1094,7 @@
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.27087291536011382</v>
+        <v>0.14663133061854361</v>
       </c>
       <c r="N6" s="7">
         <v>0.6576754830814584</v>
@@ -893,7 +1149,7 @@
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="5"/>
-        <v>0.21914999360922105</v>
+        <v>0.17245686923777293</v>
       </c>
       <c r="N7" s="7">
         <v>0.71568519429429844</v>
@@ -948,7 +1204,7 @@
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="5"/>
-        <v>0.54705515645745284</v>
+        <v>0.75038879077857168</v>
       </c>
       <c r="N8" s="7">
         <v>5.2850028046014241E-2</v>
@@ -1003,7 +1259,7 @@
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="5"/>
-        <v>6.1692000365542787E-2</v>
+        <v>0.81383527930006994</v>
       </c>
       <c r="N9" s="7">
         <v>0.21308809860812472</v>
@@ -1058,7 +1314,7 @@
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="5"/>
-        <v>9.0231723437280253E-2</v>
+        <v>0.97217812615683163</v>
       </c>
       <c r="N10" s="7">
         <v>0.82709017219206349</v>
@@ -1112,7 +1368,7 @@
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="5"/>
-        <v>4.2081526364796895E-2</v>
+        <v>4.9225743878126837E-2</v>
       </c>
       <c r="N11" s="7">
         <v>0.31858018787723441</v>
@@ -1166,7 +1422,7 @@
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="5"/>
-        <v>0.54477229114106385</v>
+        <v>0.70129233178533568</v>
       </c>
       <c r="N12" s="7">
         <v>4.9441714832939354E-2</v>
@@ -1220,7 +1476,7 @@
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="5"/>
-        <v>0.31408475820645909</v>
+        <v>0.89753572127169401</v>
       </c>
       <c r="N13" s="7">
         <v>9.0789275175559458E-2</v>
@@ -1274,7 +1530,7 @@
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="5"/>
-        <v>0.65632550071681184</v>
+        <v>0.40669454850368369</v>
       </c>
       <c r="N14" s="7">
         <v>0.31354481400876677</v>
@@ -1329,7 +1585,7 @@
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="5"/>
-        <v>0.64727981665544398</v>
+        <v>0.89702916034688307</v>
       </c>
       <c r="N15" s="7">
         <v>0.20618208392437076</v>
@@ -1387,7 +1643,7 @@
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="5"/>
-        <v>0.1797467761706929</v>
+        <v>0.6002511759655802</v>
       </c>
       <c r="N16" s="7">
         <v>0.39953080131459351</v>
@@ -1445,7 +1701,7 @@
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="5"/>
-        <v>0.54217069127992767</v>
+        <v>0.14512659326415855</v>
       </c>
       <c r="N17" s="7">
         <v>0.40484968853932757</v>
@@ -1503,7 +1759,7 @@
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="5"/>
-        <v>0.49709600223503925</v>
+        <v>0.34570983335000638</v>
       </c>
       <c r="N18" s="7">
         <v>0.33741213629515332</v>
@@ -1561,7 +1817,7 @@
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48321494814614085</v>
+        <v>0.80360607732830991</v>
       </c>
       <c r="N19" s="7">
         <v>0.27644326351109294</v>
@@ -1619,7 +1875,7 @@
       </c>
       <c r="M20">
         <f t="shared" ca="1" si="5"/>
-        <v>0.8298033768729397</v>
+        <v>0.2064879223657714</v>
       </c>
       <c r="N20" s="7">
         <v>0.95355225691916257</v>
@@ -1677,7 +1933,7 @@
       </c>
       <c r="M21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.66000007628568658</v>
+        <v>0.82406292762708189</v>
       </c>
       <c r="N21" s="7">
         <v>0.49780031450639206</v>
@@ -1735,7 +1991,7 @@
       </c>
       <c r="M22">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48504906969220218</v>
+        <v>0.55110499302905258</v>
       </c>
       <c r="N22" s="7">
         <v>0.99777944707987265</v>
@@ -1793,7 +2049,7 @@
       </c>
       <c r="M23">
         <f t="shared" ca="1" si="5"/>
-        <v>0.58357644330838987</v>
+        <v>0.97655765652561699</v>
       </c>
       <c r="N23" s="7">
         <v>0.34133183575900727</v>
@@ -1851,7 +2107,7 @@
       </c>
       <c r="M24">
         <f t="shared" ca="1" si="5"/>
-        <v>0.21152602070343141</v>
+        <v>0.22834311117219641</v>
       </c>
       <c r="N24" s="7">
         <v>0.53002196191416406</v>
@@ -1909,7 +2165,7 @@
       </c>
       <c r="M25">
         <f t="shared" ca="1" si="5"/>
-        <v>0.25338054335047955</v>
+        <v>0.17269760611099905</v>
       </c>
       <c r="N25" s="7">
         <v>0.59781950223764457</v>
@@ -1967,7 +2223,7 @@
       </c>
       <c r="M26">
         <f t="shared" ca="1" si="5"/>
-        <v>0.64275185127246992</v>
+        <v>0.69314024348779768</v>
       </c>
       <c r="N26" s="7">
         <v>0.35425136900246146</v>
@@ -2025,7 +2281,7 @@
       </c>
       <c r="M27">
         <f t="shared" ca="1" si="5"/>
-        <v>0.92615542486428348</v>
+        <v>0.31948754835505822</v>
       </c>
       <c r="N27" s="7">
         <v>0.87052133070268678</v>
@@ -2083,7 +2339,7 @@
       </c>
       <c r="M28">
         <f t="shared" ca="1" si="5"/>
-        <v>4.9911112259633628E-2</v>
+        <v>0.32328376965962291</v>
       </c>
       <c r="N28" s="7">
         <v>0.85666535883446049</v>
@@ -2141,7 +2397,7 @@
       </c>
       <c r="M29">
         <f t="shared" ca="1" si="5"/>
-        <v>0.34672000307251893</v>
+        <v>1.1843933669789863E-2</v>
       </c>
       <c r="N29" s="7">
         <v>0.40060425890931561</v>
@@ -2199,7 +2455,7 @@
       </c>
       <c r="M30">
         <f t="shared" ca="1" si="5"/>
-        <v>0.28389266659700119</v>
+        <v>0.40905257753047208</v>
       </c>
       <c r="N30" s="7">
         <v>0.32058727942291576</v>
@@ -2257,7 +2513,7 @@
       </c>
       <c r="M31">
         <f t="shared" ca="1" si="5"/>
-        <v>0.40215984172991903</v>
+        <v>0.66467891118123634</v>
       </c>
       <c r="N31" s="7">
         <v>0.13760252597132794</v>
@@ -2316,7 +2572,7 @@
       </c>
       <c r="M32">
         <f t="shared" ca="1" si="5"/>
-        <v>0.22902437988893631</v>
+        <v>0.21021956016959975</v>
       </c>
       <c r="N32" s="7">
         <v>0.11275382012540103</v>
@@ -2378,7 +2634,7 @@
       </c>
       <c r="M33">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48274538088819974</v>
+        <v>0.93276688368763927</v>
       </c>
       <c r="N33" s="7">
         <v>0.70878438486920547</v>
@@ -2440,7 +2696,7 @@
       </c>
       <c r="M34">
         <f t="shared" ca="1" si="5"/>
-        <v>0.32200256986247522</v>
+        <v>0.69468192296036246</v>
       </c>
       <c r="N34" s="7">
         <v>0.61992022851264861</v>
@@ -2502,7 +2758,7 @@
       </c>
       <c r="M35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.68283681423309806</v>
+        <v>0.65278344345818218</v>
       </c>
       <c r="N35" s="7">
         <v>0.30876621929633052</v>
@@ -2564,7 +2820,7 @@
       </c>
       <c r="M36">
         <f t="shared" ca="1" si="5"/>
-        <v>0.72686241666615603</v>
+        <v>0.5807448119811166</v>
       </c>
       <c r="N36" s="7">
         <v>0.63337685198477589</v>
@@ -2626,7 +2882,7 @@
       </c>
       <c r="M37">
         <f t="shared" ca="1" si="5"/>
-        <v>0.21676646312889114</v>
+        <v>0.81238242749041978</v>
       </c>
       <c r="N37" s="7">
         <v>0.58308396017811348</v>
@@ -2688,7 +2944,7 @@
       </c>
       <c r="M38">
         <f t="shared" ca="1" si="5"/>
-        <v>0.52527612647458322</v>
+        <v>0.41767122206475071</v>
       </c>
       <c r="N38" s="7">
         <v>0.45021574197405823</v>
@@ -2750,7 +3006,7 @@
       </c>
       <c r="M39">
         <f t="shared" ca="1" si="5"/>
-        <v>0.24302784521464615</v>
+        <v>0.47043817567812662</v>
       </c>
       <c r="N39" s="7">
         <v>0.2205184932163673</v>
@@ -2812,7 +3068,7 @@
       </c>
       <c r="M40">
         <f t="shared" ca="1" si="5"/>
-        <v>0.1996177931355686</v>
+        <v>0.85006859736813523</v>
       </c>
       <c r="N40" s="7">
         <v>0.30204449462085692</v>
@@ -2874,7 +3130,7 @@
       </c>
       <c r="M41">
         <f t="shared" ca="1" si="5"/>
-        <v>0.73563297522819904</v>
+        <v>8.9696273729848897E-2</v>
       </c>
       <c r="N41" s="7">
         <v>0.96960269632308016</v>
@@ -2936,7 +3192,7 @@
       </c>
       <c r="M42">
         <f t="shared" ca="1" si="5"/>
-        <v>0.5889211263879971</v>
+        <v>0.88484789349025561</v>
       </c>
       <c r="N42" s="7">
         <v>0.64894817609047195</v>
@@ -2998,7 +3254,7 @@
       </c>
       <c r="M43">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48080236561476353</v>
+        <v>0.2428576431436591</v>
       </c>
       <c r="N43" s="7">
         <v>0.9671384975591113</v>
@@ -3060,7 +3316,7 @@
       </c>
       <c r="M44">
         <f t="shared" ca="1" si="5"/>
-        <v>8.7633790277564794E-2</v>
+        <v>0.27389857288086694</v>
       </c>
       <c r="N44" s="7">
         <v>0.16728056449427242</v>
@@ -3122,7 +3378,7 @@
       </c>
       <c r="M45">
         <f t="shared" ca="1" si="5"/>
-        <v>0.38953992059987053</v>
+        <v>0.83201927618557681</v>
       </c>
       <c r="N45" s="7">
         <v>0.97014034368482205</v>
@@ -3184,7 +3440,7 @@
       </c>
       <c r="M46">
         <f t="shared" ca="1" si="5"/>
-        <v>0.87290853938821289</v>
+        <v>0.87645142457564595</v>
       </c>
       <c r="N46" s="7">
         <v>0.14184237276812373</v>
@@ -3246,7 +3502,7 @@
       </c>
       <c r="M47">
         <f t="shared" ca="1" si="5"/>
-        <v>0.86083838775486099</v>
+        <v>0.90854311938304544</v>
       </c>
       <c r="N47" s="7">
         <v>0.87369324209203869</v>
@@ -3308,7 +3564,7 @@
       </c>
       <c r="M48">
         <f t="shared" ca="1" si="5"/>
-        <v>0.61368150877478844</v>
+        <v>0.39640853400030152</v>
       </c>
       <c r="N48" s="7">
         <v>0.23215110927673421</v>
@@ -3370,7 +3626,7 @@
       </c>
       <c r="M49">
         <f t="shared" ca="1" si="5"/>
-        <v>0.54441713376573075</v>
+        <v>0.57156525170877459</v>
       </c>
       <c r="N49" s="7">
         <v>0.41140424416952115</v>
@@ -3431,7 +3687,7 @@
       </c>
       <c r="M50">
         <f t="shared" ca="1" si="5"/>
-        <v>0.56051961197523403</v>
+        <v>0.48766084307206592</v>
       </c>
       <c r="N50" s="7">
         <v>0.45922463930133517</v>
@@ -3493,7 +3749,7 @@
       </c>
       <c r="M51">
         <f t="shared" ca="1" si="5"/>
-        <v>0.65148718221848223</v>
+        <v>0.99804456934474717</v>
       </c>
       <c r="N51" s="7">
         <v>0.27298193365189094</v>
@@ -3555,7 +3811,7 @@
       </c>
       <c r="M52">
         <f t="shared" ca="1" si="5"/>
-        <v>0.32144022415323315</v>
+        <v>0.63570733506099186</v>
       </c>
       <c r="N52" s="7">
         <v>0.90367281274799927</v>
@@ -3617,7 +3873,7 @@
       </c>
       <c r="M53">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48874634719856203</v>
+        <v>0.85527024528919049</v>
       </c>
       <c r="N53" s="7">
         <v>0.33401603606125274</v>
@@ -3681,7 +3937,7 @@
       </c>
       <c r="M54">
         <f t="shared" ca="1" si="5"/>
-        <v>0.15415448002016974</v>
+        <v>0.10550790254266351</v>
       </c>
       <c r="N54" s="7">
         <v>0.78782993494586073</v>
@@ -3743,7 +3999,7 @@
       </c>
       <c r="M55">
         <f t="shared" ca="1" si="5"/>
-        <v>0.28764823460172417</v>
+        <v>0.4895368809113485</v>
       </c>
       <c r="N55" s="7">
         <v>0.32262435562402192</v>
@@ -3805,7 +4061,7 @@
       </c>
       <c r="M56">
         <f t="shared" ca="1" si="5"/>
-        <v>0.66970221502585592</v>
+        <v>0.2433873111981758</v>
       </c>
       <c r="N56" s="7">
         <v>0.91897761332231853</v>
@@ -3867,7 +4123,7 @@
       </c>
       <c r="M57">
         <f t="shared" ca="1" si="5"/>
-        <v>0.78956044038328421</v>
+        <v>5.6128331407171994E-2</v>
       </c>
       <c r="N57" s="7">
         <v>0.29246561980543551</v>
@@ -3929,7 +4185,7 @@
       </c>
       <c r="M58">
         <f t="shared" ca="1" si="5"/>
-        <v>0.78363713904584875</v>
+        <v>0.43566184175013289</v>
       </c>
       <c r="N58" s="7">
         <v>0.74772967135635671</v>
@@ -3991,7 +4247,7 @@
       </c>
       <c r="M59">
         <f t="shared" ca="1" si="5"/>
-        <v>0.8569611962468684</v>
+        <v>0.83774986123159034</v>
       </c>
       <c r="N59" s="7">
         <v>0.69621562359731126</v>
@@ -4053,7 +4309,7 @@
       </c>
       <c r="M60">
         <f t="shared" ca="1" si="5"/>
-        <v>6.3564260943347106E-2</v>
+        <v>0.23625362423738716</v>
       </c>
       <c r="N60" s="7">
         <v>0.20909957463594775</v>
@@ -4115,7 +4371,7 @@
       </c>
       <c r="M61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.47283574867453626</v>
+        <v>0.59432015021307294</v>
       </c>
       <c r="N61" s="7">
         <v>0.79346297452888637</v>
@@ -4177,7 +4433,7 @@
       </c>
       <c r="M62">
         <f t="shared" ca="1" si="5"/>
-        <v>0.15064503285698461</v>
+        <v>0.86171562639225241</v>
       </c>
       <c r="N62" s="7">
         <v>0.31149909990883551</v>
@@ -4239,7 +4495,7 @@
       </c>
       <c r="M63">
         <f t="shared" ca="1" si="5"/>
-        <v>0.83118432774567241</v>
+        <v>0.32427284585438865</v>
       </c>
       <c r="N63" s="7">
         <v>0.48031537986172113</v>
@@ -4301,7 +4557,7 @@
       </c>
       <c r="M64">
         <f t="shared" ca="1" si="5"/>
-        <v>0.11157450195642737</v>
+        <v>0.68586710422953667</v>
       </c>
       <c r="N64" s="7">
         <v>0.80102559709529053</v>
@@ -4363,7 +4619,7 @@
       </c>
       <c r="M65">
         <f t="shared" ca="1" si="5"/>
-        <v>0.57834646522794808</v>
+        <v>0.26474148815421039</v>
       </c>
       <c r="N65" s="7">
         <v>0.28828332955544012</v>
@@ -4425,7 +4681,7 @@
       </c>
       <c r="M66">
         <f t="shared" ca="1" si="5"/>
-        <v>0.84508262240448895</v>
+        <v>0.83764455756455691</v>
       </c>
       <c r="N66" s="7">
         <v>0.48899291055505756</v>
@@ -4487,7 +4743,7 @@
       </c>
       <c r="M67">
         <f t="shared" ref="M67:M72" ca="1" si="15">RAND()</f>
-        <v>0.71393714410640696</v>
+        <v>0.13355044577160824</v>
       </c>
       <c r="N67" s="7">
         <v>0.80047770738788393</v>
@@ -4549,7 +4805,7 @@
       </c>
       <c r="M68">
         <f t="shared" ca="1" si="15"/>
-        <v>0.25805081030714794</v>
+        <v>7.5304253480975802E-2</v>
       </c>
       <c r="N68" s="7">
         <v>0.46632345703033884</v>
@@ -4611,7 +4867,7 @@
       </c>
       <c r="M69">
         <f t="shared" ca="1" si="15"/>
-        <v>0.84915831308132106</v>
+        <v>0.17999744541827212</v>
       </c>
       <c r="N69" s="7">
         <v>0.74207184365936485</v>
@@ -4673,7 +4929,7 @@
       </c>
       <c r="M70">
         <f t="shared" ca="1" si="15"/>
-        <v>4.553528136569851E-2</v>
+        <v>0.27298981319065307</v>
       </c>
       <c r="N70" s="7">
         <v>0.96530053340657029</v>
@@ -4735,7 +4991,7 @@
       </c>
       <c r="M71">
         <f t="shared" ca="1" si="15"/>
-        <v>0.93147627820709455</v>
+        <v>0.63911660520598434</v>
       </c>
       <c r="N71" s="7">
         <v>0.12934481239966189</v>
@@ -4797,7 +5053,7 @@
       </c>
       <c r="M72">
         <f t="shared" ca="1" si="15"/>
-        <v>0.27893429398140956</v>
+        <v>0.69912305740245761</v>
       </c>
       <c r="N72" s="7">
         <v>0.14921015862555653</v>
@@ -4860,7 +5116,7 @@
       </c>
       <c r="M73">
         <f t="shared" ref="M73:M86" ca="1" si="18">RAND()</f>
-        <v>0.87585954797346188</v>
+        <v>0.63410041249725368</v>
       </c>
       <c r="N73" s="7">
         <v>8.1118040046405104E-2</v>
@@ -4923,7 +5179,7 @@
       </c>
       <c r="M74">
         <f t="shared" ca="1" si="18"/>
-        <v>0.75808963133160756</v>
+        <v>0.22476161112553228</v>
       </c>
       <c r="N74" s="7">
         <v>0.17936155117592445</v>
@@ -4986,7 +5242,7 @@
       </c>
       <c r="M75">
         <f t="shared" ca="1" si="18"/>
-        <v>0.43471890677805147</v>
+        <v>5.6044546051217448E-2</v>
       </c>
       <c r="N75" s="7">
         <v>0.39247141670469787</v>
@@ -5049,7 +5305,7 @@
       </c>
       <c r="M76">
         <f t="shared" ca="1" si="18"/>
-        <v>0.69796014017768948</v>
+        <v>0.57200641089936521</v>
       </c>
       <c r="N76" s="7">
         <v>0.45266156241192723</v>
@@ -5112,7 +5368,7 @@
       </c>
       <c r="M77">
         <f t="shared" ca="1" si="18"/>
-        <v>0.2967084358170281</v>
+        <v>0.30754813071969633</v>
       </c>
       <c r="N77" s="7">
         <v>0.16334533433755671</v>
@@ -5175,7 +5431,7 @@
       </c>
       <c r="M78">
         <f t="shared" ca="1" si="18"/>
-        <v>0.86051208612595032</v>
+        <v>2.2300089389511668E-2</v>
       </c>
       <c r="N78" s="7">
         <v>0.52468795773904264</v>
@@ -5238,7 +5494,7 @@
       </c>
       <c r="M79">
         <f t="shared" ca="1" si="18"/>
-        <v>0.2790378929751639</v>
+        <v>0.8363705662005646</v>
       </c>
       <c r="N79" s="7">
         <v>0.63253074449134639</v>
@@ -5301,7 +5557,7 @@
       </c>
       <c r="M80">
         <f t="shared" ca="1" si="18"/>
-        <v>0.77003222666615934</v>
+        <v>0.56118901456828363</v>
       </c>
       <c r="N80" s="7">
         <v>0.69296323757560652</v>
@@ -5364,7 +5620,7 @@
       </c>
       <c r="M81">
         <f t="shared" ca="1" si="18"/>
-        <v>0.23307429674518765</v>
+        <v>0.75198027249384292</v>
       </c>
       <c r="N81" s="7">
         <v>0.29589698897676608</v>
@@ -5427,7 +5683,7 @@
       </c>
       <c r="M82">
         <f t="shared" ca="1" si="18"/>
-        <v>0.75014099611025808</v>
+        <v>0.89382043863083904</v>
       </c>
       <c r="N82" s="7">
         <v>0.77516020799779406</v>
@@ -5490,7 +5746,7 @@
       </c>
       <c r="M83">
         <f t="shared" ca="1" si="18"/>
-        <v>0.93675223011444908</v>
+        <v>0.49820276399712637</v>
       </c>
       <c r="N83" s="7">
         <v>0.4658991273440577</v>
@@ -5553,7 +5809,7 @@
       </c>
       <c r="M84">
         <f t="shared" ca="1" si="18"/>
-        <v>5.8306383940534889E-2</v>
+        <v>0.48941257595578203</v>
       </c>
       <c r="N84" s="7">
         <v>0.72317574723917522</v>
@@ -5616,7 +5872,7 @@
       </c>
       <c r="M85">
         <f t="shared" ca="1" si="18"/>
-        <v>0.75155605234550582</v>
+        <v>3.4414544392775692E-2</v>
       </c>
       <c r="N85" s="7">
         <v>0.87006243512491854</v>
@@ -5679,7 +5935,7 @@
       </c>
       <c r="M86">
         <f t="shared" ca="1" si="18"/>
-        <v>0.7095419407886232</v>
+        <v>0.40816162575553294</v>
       </c>
       <c r="N86" s="7">
         <v>0.87611417886010456</v>
@@ -5704,4 +5960,444 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD59DFE-7F75-4DF4-B32D-CE7E758F39E4}">
+  <dimension ref="A1:A85"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>